<commit_message>
Added 'Available Routes' and 'Postman Requests' documents and updated the Hour log
</commit_message>
<xml_diff>
--- a/documents/DTT-Test-Hour-Log.xlsx
+++ b/documents/DTT-Test-Hour-Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abuhn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\intern-dtt\test proj\internDTT\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9C5B43D-22DE-4A98-AB4C-A17E5BB21F82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3DD396-E712-4A1C-BCA5-AAD759306A84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Subject</t>
   </si>
@@ -128,6 +128,36 @@
   </si>
   <si>
     <t>Reading of requirements and user stories, paper planning the database tables, structure, needed requests.</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>Eliminate Repetitiveness</t>
+  </si>
+  <si>
+    <t>Fixing of specific functions</t>
+  </si>
+  <si>
+    <t>Complete setup of the router for Listings, Houses, Rooms and Users</t>
+  </si>
+  <si>
+    <t>Replace declaration of Request and Response in every Controller. Controllers inherit from BaseController instead of Mvc/Controller. View is disabled in BaseController before execution, instead of every function in every controller. Added an extra function in Controller Base.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renamed functions and variables that had unproper naming. Removed commented code, corrected comments that had wrong information (e.g. mentioning the user when creating a new house). </t>
+  </si>
+  <si>
+    <t>Comments/ variables fixing</t>
+  </si>
+  <si>
+    <t>Replaced 'findFirst(id = ?)' with 'findFirstById(?)'. ControllerBase has the 'errorCheck' function. When the check is passed a generic response message is given.</t>
+  </si>
+  <si>
+    <t>Extra Documentation</t>
+  </si>
+  <si>
+    <t>Added Router documentation and Postman JSON file. Readme file contains more information.</t>
   </si>
 </sst>
 </file>
@@ -1733,7 +1763,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1909,42 +1939,82 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="18">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19">
+        <v>44353</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="18">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19">
+        <v>44353</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="18">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19">
+        <v>44353</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="16"/>
+      <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19">
+        <v>44353</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="18">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19">
+        <v>44354</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
@@ -2058,7 +2128,7 @@
       </c>
       <c r="B30" s="15">
         <f>SUM(B4:B28)</f>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>

</xml_diff>